<commit_message>
Get daily reddit data: Tue Jan 23 08:08:59 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C448"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5550,6 +5550,2505 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>19dj078</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>Did my right hand last night, love the colors!</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgt2yxgh75ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>19di6dq</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t>Recommendation for nail sticker brands?</t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19di6dq/recommendation_for_nail_sticker_brands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>19dhkbr</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t>Manucurist Green Flash First Impression/Early Review</t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dhkbr/manucurist_green_flash_first_impressionearly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>19dhl9p</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Gaint hands lol</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9mpibbz2r4ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>19dhg4h</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>fav shape?</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dhg4h</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>19dh2cp</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Can't take my eyes off my nails😍</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ro9ibs1g4ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>19df2d7</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t>My gel nails always lift from the bottom</t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19df2d7/my_gel_nails_always_lift_from_the_bottom/</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>19dg42s</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink and black shorties </t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/al2812ltb4ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>19dg0j5</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Removal or refill?</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dg0j5</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>19dficr</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>What is your go to top coat?</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dficr/what_is_your_go_to_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>19dfcpv</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>I am struggling with my nail art lines 😤</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9suqxqdf44ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>19dfbag</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>MANicure</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lu669qq144ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>19df7v0</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>When your vision doesn’t translate. Not sure I like them</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5wpdwo434ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>19df7ic</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>New nails!</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19df7ic</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>19dd6ur</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Unpopular Opinion: Acrylic nails irritate me. It’s like removing a bra when you take them off. I’ll be pleased with gel polish, that’s all.</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ru6kzaltk3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>19dbehn</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>OPI gel on my real nails</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dbehn</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>19deggn</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>ILNP</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gjzgu1m1w3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>19deb48</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Can I ask for a color change as part of an acrylic infill?</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19deb48/can_i_ask_for_a_color_change_as_part_of_an/</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>19ddb91</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>I’ve been working on my decal skills lately.</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fci3p5exl3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>19dd8aj</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>First nails of 2024</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wv0mmgg6l3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>19dcxy8</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>It's almost here!</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t71p8sipi3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>19dcvh5</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Tried marbling tonight</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h6a4s3d3i3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>19dccl5</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Going into Valentine’s unexpectedly single…but at least my nails are cute!</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1gdsh6zid3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>19dca5o</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>French mani pedi</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dca5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>19dc7c4</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t>Went in wanting dark and ombré….kind of loving my accidental Hades vibe</t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dc7c4</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>19dbz29</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>I accidentally used top coat instead of my builder gel to attach my full tips.</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nyqa05faa3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>19dayay</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t>First Time Getting Nails Done 😸</t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dayay</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>19dav0c</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Romantic nails</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dav0c</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>19damh8</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>Valentines Designs</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19damh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>19dabfr</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>polygel help!</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dabfr/polygel_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>19da52l</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>did these myself, so happy with them!</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dol90w7kv2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>19d8ya9</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>When he’s a red flag but red is my fave color 😝❤️</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mp0xapkim2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>19d8wtc</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t>Deep reddish brown</t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d8wtc</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>19d825m</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>attack titan freehand!</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/32i0ho0vf2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>19d6uox</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t>Hard Gel (ibd clear)</t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k9mz6kfa72ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>19d6rmz</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>My simpler look after the holiday glitter ✨</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d6rmz</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>19d5zm0</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What I got vs what I wanted (inspo IG @_pgoo)</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d5zm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>19d5c97</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>New nails</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3yvwn2icw1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>19d4vgt</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>Mani of the Week</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4vgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>19d4sca</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>Press on nail before/after</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4sca</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>19d4l09</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t>Another Set of Valentine’s Nails 🩷🌸🤍</t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4l09</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>19d2yz1</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>post acrylic nails :/</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d2yz1</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>19d66sw</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t>Wide nail acrylics?</t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19d66sw/wide_nail_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>19d651d</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>We are looking at the end of week 3🎉</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yiuld3b822ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>19czhqo</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Crescent City inspired nails!</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19czhqo</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>19d5wc3</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>Just a simple French with a bow 🎀</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7u8m9usf02ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>19cwemj</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19cwemj/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>19d5le8</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Will using nail glue with gel strips help them not pop off?</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19d5le8/will_using_nail_glue_with_gel_strips_help_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>19d4wu3</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Anyone else have a sweet tooth?</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4wu3</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>19d4p2v</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>JJK theme</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4p2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>19d4nnq</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t>Practicing my gel art skills 🥰</t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4nnq</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>19d3v6p</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t>Can gel nails help protect your nails from breaking</t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19d3v6p/can_gel_nails_help_protect_your_nails_from/</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>19d3riq</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>My birthday nails</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d3riq</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>19d3qc0</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>When you let your nail tech decide. Love this set!</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7vjbxyzek1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>19d3asu</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t>Nails with bestie 💖</t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/knfxyyv7h1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>19d35xw</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>Color advice please?</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ebktsg7g1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>19d2p7p</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Nails of the week 🎀</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d2p7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>19d2fgc</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t>Would you like a subtle glazed green set? I tried my best! 🌿 (◍´ᯅ `◍)</t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d2fgc</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>19d15d4</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>In love with these sets. Those checkers took me multiple days lol!</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v0pfbm3p11ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>19d12wa</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>New mani! ✨️🌙</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d12wa</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>19d0tbk</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>what’s the strongest way to do my nails?</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19d0tbk/whats_the_strongest_way_to_do_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>19d037e</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t>Can I use reuglar glue with the btartbox X Coat tips?</t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19d037e/can_i_use_reuglar_glue_with_the_btartbox_x_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>19cz2if</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t>Praise for my nail tech</t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cz2if</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>19cyncv</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>How to get rid of bumps</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pmgh5kq9j0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>19cxqab</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>Uv gel stickers suggestions</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19cxqab/uv_gel_stickers_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>19cxpn6</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>I did my sisters engagement nails. Check out that ring! White and yellow diamonds</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7dxr88gvb0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>19cwog7</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>self-taught nail art progress</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cwog7</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>19cwiuk</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>One of my favorite set ✨</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p9xdcdox10ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>19cvx35</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Baby boomer 💅🏼</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f4ta1n6rwzdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>19cviht</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2q2fp490tzdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>19cv07q</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>recently started doing a bit of nail art myself</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cv07q</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>19culrt</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Acrylic extensions without polish so I can paint them myself at home. £25 Manchester, UK!</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rs6tf00yjzdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>19cug92</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>marble nails with silver chrome 💙🤎</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cug92</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>19csvfv</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>My new favourites 💜 Used soft gel tips for the first time, is there any going back? 😳</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19csvfv</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>19csoln</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>Shorties</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19csoln</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>19csn09</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>Which brands do you guys recommend for cat eye nail polish/gel?</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19csn09/which_brands_do_you_guys_recommend_for_cat_eye/</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>19crc0r</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>First Set Ever!</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19crc0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>19cr8p6</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>New cursed pose: The Reach-around</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mzzxz0efydc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>19cr6hg</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t>I love being a woman</t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cr6hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>19cqvxu</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>I love snoopy 💗</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nw3g55gpaydc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>19di8rb</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Great customer service shout out</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19di8rb/great_customer_service_shout_out/</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>19di66t</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>How do I keep press ons on better?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19di66t/how_do_i_keep_press_ons_on_better/</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>19dh1oa</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>alien invasion 👽</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dh1oa</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>19dfbfz</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Dip powder has ruined my nails — help</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87tav4l244ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>19df42f</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Fishing lure nails! :)</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19df42f</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>19dela2</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>I want this color soo bad.</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yv90j40cx3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>19ddeze</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>Frenchie mani pedi</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ddeze</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>19dbxkj</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Look out friends, new magnet hack coming in hot</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dbxkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>19das02</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>So glowy!</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bzhj86h03ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>19dany1</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Beautiful shade but on me just looks off, idk why... Finishing my swatches of this collection! - Kiko Milano Perfect Gel shade #119 🩵 💅🏻</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dany1</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>19daau8</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>What are the tricks to using chrome powders/chrome powder pen?</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19daau8/what_are_the_tricks_to_using_chrome_powderschrome/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>19d9zn8</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>Messing around with stamping and chrome powder</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lnd6k4tcu2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>19d9z9q</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Orly - Mirror Mirror</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d9z9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>19d9ycs</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Earth to Gaia by Mooncat</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d9ycs</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>19d9p8o</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>How It Started vs How It's Going</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d9p8o</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>19d9otl</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Help with gel nails!</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19d9otl/help_with_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>19d941q</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>My most beautiful iridescent ever! Even my professor complemented me on it while I was trying not to melt it from the Benson burner.</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d941q</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>19d8tpb</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Le Mini Macaron - Sugar Stone</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/27w7mlokl2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>19d8rku</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Mooncat a doll's house is such a pretty neutral</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg4jdv65l2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>19d8mpw</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Celestial stamping practise (while I wait for more colours than B&amp;W)</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d8mpw</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>19d88iw</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>White spot on pinky</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6hhxnzh6h2ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>19d7sog</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>♒ Aquarius Szn Birthday Mani (from an elder Millennial)</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d7sog</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>19d6luh</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>My simpler look after the holiday glitter</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d6luh</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>19d2wlg</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Nails still brittle after Strengthener !</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19d2wlg/nails_still_brittle_after_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>19d5xa7</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Sheen Queen 👊</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zlbqsrtm02ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>19cy28g</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Alchemy Lacquers Spanish Shawl</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7rxwbk4ne0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>19d5nnk</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>And the shadows flee away - A England</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d5nnk</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>19d4vo7</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Charging for basic Polish</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19d4vo7/charging_for_basic_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>19d4jav</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>Tutorial for the paper clip heart magnet trick!</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h3q9amlbq1ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>19d4dsa</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Soaking to remove glitter</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4dsa</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>19d3ksf</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>My accidental early Valentine's Day nails that I keep getting distracted by</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo7op5b9j1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>19d3hcs</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Does this happen to anyone else?</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4jqonbchi1ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>19d3fvp</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>First DIY polish (SolarGlowThermal)</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d3fvp</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>19d2yfp</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Ouzle Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d2yfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>19d28c3</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t>Been trying to grow out this break since OCTOBER.</t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d28c3</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>19d27xj</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>base coat recommendations</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19d27xj/base_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>19d21r1</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t>Tamiah 🩷✨</t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d21r1</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>19d11tg</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>PLEASE HELP! My polish always pops off in one single piece and I have no clue what I am doing wrong, more info in comments</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rl2bo3q011ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>19d0u7f</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Zoya Inez is bringing me so much joy!</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdfjwbvhz0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>19d03yw</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t>This polish is six years old</t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqm55g87u0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>19czhig</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>GLOWY polish recs? Obsessed with these polishes with a blue or pink glow to them. (Pics just for reference only)</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19czhig</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>19cz7se</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Beginner: Zoya Clarice</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3mkg0y5ln0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>19cz6db</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>🌼🪻Pansies🪻🌼</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cz6db</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>19cynfx</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>Did I do crackle wrong? Or is this how is supposed to look? I thought it was going to be more fine lines. Maybe I did it too thick or thin???</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ift0fdeaj0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>19cyjvg</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t>Finally got around to trying Fishnet Stockings 😍</t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx8scg7ii0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>19cxngu</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t>Black Pearl</t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cxngu</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>19cx6yl</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>Snow and Violets by Shleee Polish</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cx6yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>19cx4nm</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Wherever you Dwell</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19cx4nm</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>19cx0lv</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>ILNP Be Mine</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49v5fnv460ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>19cwxco</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>Comparison request</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19cwxco/comparison_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>19cwo2w</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Haven’t posted in years, just got back into it.</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p0oxp37530ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>19cwnz8</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Finding the thermals at Nailland</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19cwnz8/finding_the_thermals_at_nailland/</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>19ct5to</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t>Orly Color Pass Spring 2024 — Morning Dew</t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1mx1sty54zdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>19ct4sz</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19ct4sz/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>19crcqm</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>Love how futuristic this colour is!</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zdpp7o4vgydc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>19djbpw</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t xml:space="preserve">"simple" holdover til Valentine's </t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cpw2117jb5ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>19dhv8w</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>My set this week</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxctvb45u4ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>19dfl16</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>freehanded these, proud of how they turned out!</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/we7jz16l64ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>19dc97d</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Progress! Left is week 2 of painting my own nails, right is one year</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/io855pwpc3ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>19d4jxx</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t>I'm practicing my gel art skills 🥰</t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d4jxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>19d2qio</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Nails of the week 🎀</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d2qio</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>19d0vxu</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Demon Slayer nails!</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19d0vxu</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>19d0uhw</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>💗 Valentine’s Day Nail Art 💗</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0djyn47jz0ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>19cxqhv</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t>My uncle overcame his fragile masculinity and let me paint one nail</t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjngv3r2c0ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>19cvi59</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>💙</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tqcox83xszdc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>19csx48</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>My new favourite set 💜 Used soft gel tips for the first time, is there any going back? 😳</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19csx48</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>19crmqa</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>nightmare before christmas set i did back in december 😍</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yin7zuhkydc1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 24 08:08:26 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C448"/>
+  <dimension ref="A1:C606"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8049,6 +8049,2692 @@
         </is>
       </c>
     </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>19ebwm6</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>I just started doing my nails at home and wanted to try out dual forms. Should I try full cover dual forms or dual form tips? which one of them is beginner-friendly? And can I do aquarium nails with dual forms too?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ebwm6/i_just_started_doing_my_nails_at_home_and_wanted/</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>19ebu0i</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Kitty Kitty 🌸</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6alilo6ybcec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>19ebkiq</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>I get a little gap between my real nail and the fake nail sometimes</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ebkiq/i_get_a_little_gap_between_my_real_nail_and_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>19eaica</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>Wanted romeo and juliet nails (movie ofc!)</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eaica</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>19eamkq</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Best holographic and chameleon gel polishes</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbpf083h0cec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>19eagi1</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>New galaxy set</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eagi1</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>19ea51k</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>Care/styling tips for short nails?</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ea51k</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>19e7x21</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>Pls help</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7tl4bk509bec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>19e388n</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>February nails</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/espc0pqk4aec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>19e8miw</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Just got fake nails for the first time as a guy what does Reddit think</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/40aql9wtfbec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>19e8byj</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>My latest favs!</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e8byj</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>19e7z50</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>Black or blue?</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e7z50</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>19e7pu4</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>Ready for my tropical vacay with this set!</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ficbawm37bec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>19e7oz0</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>i’m afraid he ate …</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e7oz0</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>19e7hfh</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t>How To Groom My Nails as a Male?</t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e7hfh/how_to_groom_my_nails_as_a_male/</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>19e7ghl</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>Olive and June?</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e7ghl/olive_and_june/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>19e7cdp</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Alternatives to full gelly tips? Builder gel maybe?</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e7cdp/alternatives_to_full_gelly_tips_builder_gel_maybe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>19e6yzx</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Nails ❤️💕</t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e6yzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>19e6j8i</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My best nail ever </t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/de17itonwaec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>19e6cp1</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I have a nail question</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e6cp1/i_have_a_nail_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>19e5hlk</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Slytherin Nails 🐍</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlrgr4vpnaec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>19e5dko</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>lavender haze and velvet</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e5dko</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>19e5d2k</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>What nails suit my hands best?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e5d2k</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>19e50yo</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Press-on manicure</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/l7psft6pjaec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>19e4uij</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t>My tech always slays</t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3a8ssr6iaec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>19e4tmp</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Pink chromey sky with Cupid 💖</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e4tmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>19e4q86</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>Polish changed colour</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e4q86</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>19e47ec</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t>Suggestions on natural pink nail strengthener?</t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e47ec/suggestions_on_natural_pink_nail_strengthener/</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>19e3qn1</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t>vday set on natural nails💌</t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oslnmwdt8aec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>19e3aaj</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>they feel so romantic 🌸 perfect for spring but I love florals for any season :p</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e3aaj</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>19e1u9x</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>this color is named Fetish</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvd3pgant9ec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>19dymyh</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>This is my favorite set to get. How do you think they did?</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dymyh</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>19e188e</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t>Looking to buy handmade stick ons!</t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19e188e/looking_to_buy_handmade_stick_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>19e15qe</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>Nail art for my beloved sister</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e15qe</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>19e10m2</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>NAILS I DID TODAY!!</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e10m2</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>19e0mwr</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t>Mermaid Fantasy 🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e0mwr</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>19e0i2k</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>Love the press ons</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibmqvgymj9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>19e095h</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t>The time I tried blue and gold ✨</t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gspbydeuh9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>19e05a8</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t>Vacation-ready!</t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0wn4rhd1h9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>19dzqe9</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>:( it's just been 2 weeks</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gfi3pnzzd9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>19dzpzk</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t>Subtle Valentines Day launch</t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d4qvox5xd9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>19dz216</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>How can I improve?</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3twbhtc299ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>19dywob</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>Zebra Print</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1wn7l1fz79ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>19dyvdx</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t>Tips to paint non dominant hand</t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dyvdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>19dyeyo</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>(Update) Acrylic extensions without polish so I can paint them myself at home.</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6tv23g8b49ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>19dy8yv</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Dark, vampy vibes for vday 🖤</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dy8yv</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>19dy6bi</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Blue</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/as8e4x9j29ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>19dx72c</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t>fun soft set i did on myself !!🤍</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dx72c</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>19dv4qv</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>My nails are damaged</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dv4qv/my_nails_are_damaged/</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>19dwvgy</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t>Got bored of my velour pink nails and added a little something🩷</t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dwvgy</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>19dwr90</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t>Cat eye gel</t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5hyfmhd1s8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>19dwlep</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t>BIAB- BRATZ nail art, the purple chrome is EVERYTHING i absolutely love it, my nail tech always pushing herself 💜✨</t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jpzs1rmuq8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>19dwdec</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Valentines themed nails I did on my own!</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dwdec</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>19dw64v</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>FIRTS EVER NAIL EXTENSIONS</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iof1xqxqn8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>19dvv71</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>Tips and tricks</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dvv71/tips_and_tricks/</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>19dvkpe</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>I’ve been doing my own nails for a while but I decided to take a break and go to a nail tech. I’m super happy with it ❤️</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s2ihicldj8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>19dvc45</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>So grown out but these are too cute not to share 🥰</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/suieul4mh8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>19dv1no</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Nail Shape</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dv1no</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>19duahu</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Trying out acrylics again</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19duahu</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>19du8x6</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Such a Farse and Black the Night</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19du8x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>19dtyb8</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>Unintentionally got a really cute color</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mgypbhlr78ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>19dtiqf</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t>Heart nails</t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dtiqf</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>19dthjs</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>Eren Yeager freehand</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eoglf1ya48ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>19dt6i2</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>Which shape do you guys think suits my hands best?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dt6i2</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>19do166</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t>Tips for using the e-file</t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19do166/tips_for_using_the_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>19djifv</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>Why do my nails grow so weird?</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19djifv</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>19drkb7</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>I’m obsessed with this set I did</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19drkb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>19dqk48</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>Glue tab adhesives + soft gel nails?</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dqk48/glue_tab_adhesives_soft_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>19dppj9</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t>Is it possible to oil your nails too much?</t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dppj9/is_it_possible_to_oil_your_nails_too_much/</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>19dpgwy</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Help: how to save this manicure</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8d88lcl887ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>19dpasd</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>I'm slowly recovering from my depression and this is the first set of nails I made. I know its a bit cringe and not a big deal, but it feels awesome. What do you think?</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dpasd</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>19dp3jr</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t>Thought of these last night.. not the cleanest set but I do love them!!</t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/utt0w00157ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>19doz5n</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>Something in my blue glitter Maybelline nail varnish makes my Essie pink nail varnish get orange specks in it? Why is this?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g9vqxb0047ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>19doqcd</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>Infills</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19doqcd/infills/</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>19dodgt</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t>cleanest break ever!</t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qj3dhkaky6ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>19dn9lb</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>My nail art work on natural nails.</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzayt5lon6ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>19dltbt</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>Totally forgot to post these</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dltbt</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>19dlrmj</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Punta Cana ready.</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7yn89i6v66ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>19dlk0u</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>Got a batch order consists of 5 nail sets today</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dlk0u</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>19dkxn6</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t>Nail art pens… any good?</t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19dkxn6/nail_art_pens_any_good/</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>19dkvn5</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t>Did Valentine’s Day nails on my friend</t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8re8v6nrv5ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>19eaeuc</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t>Very similar but still quite different</t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2acfsl2sxbec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>19e9145</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>First Go at Green 💚</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e9145</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>19e8p3v</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Just got fake nails for the first time as a guy what does Reddit think</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/trro7grhgbec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>19e89qu</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t>Finally got an organization system for my polish + advice for polish ravenous newbies lol</t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e89qu/finally_got_an_organization_system_for_my_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>19e86oq</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Ohora gel strips + magnetic gel for velvet effect</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e86oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>19e7xnc</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Muted black stamping polish</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e7xnc/muted_black_stamping_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>19e7tgg</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>Impulse purchase, impulse swatches</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e7tgg</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>19e7io0</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>It's giving heat miser🔥/snow miser🥶</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e7io0</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>19e6zst</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>A England Polish</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tckpoaim0bec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>19e6src</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t>Chrome Like Nail polish w/o powder?</t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xzwhgpoyyaec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>19e6jns</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>I'm officially obsessed with Painted Polish</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e6jns</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>19e64gu</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Looking for a match</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kx8rb806taec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>19e55bx</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>My first ILNP!!!</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t6ujma7rkaec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>19e4uwa</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>ORLY BIAB - What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e4uwa/orly_biab_what_am_i_doing_wrong/</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>19e4uh9</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>Witchcult Sweater Weather</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e4uh9/witchcult_sweater_weather/</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>19e44hp</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>Favorite brands for high quality polish in solid colors?</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e44hp/favorite_brands_for_high_quality_polish_in_solid/</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>19e2udr</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t>New favorite neutral 🙌🏻</t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9xilwt9j1aec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>19e2f55</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t>Alright y’all, I want to make the switch but need the most heavy duty routines, products and advice!</t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e2f55/alright_yall_i_want_to_make_the_switch_but_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>19e1z09</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Fake OPI?</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1ic6fp5ou9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>19e1w6c</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t>Was so excited to use this color!</t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wlarxr1u9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>19e1scs</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t>Is dip at a salon ever sanitary?</t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19e1scs/is_dip_at_a_salon_ever_sanitary/</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>19dzx1f</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t>How to make my gel last</t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dzx1f/how_to_make_my_gel_last/</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>19e1cuk</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Full collection swatches for Orly - Spring 2024 - 🧜‍♀️🧜‍♂️Aqua Aura🧜‍♂️🧜‍♀️</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e1cuk</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>19e0t0l</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>Recently, whenever i am looking for Nailspo on pinterest, i get recommend pictures like this. That has to be AI or something, right? Or am i going crazy</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w2erg2xul9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>19e0i1w</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Beautiful flakies</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6sp1wy4nj9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>19dzqmh</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>Subtle Valentines Day launch</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y3psk9r1e9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>19dz7h9</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Clear pink coat 🩷</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aak5gzn6a9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>19dyrh9</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Mooncat - This Is A Storm Warning</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dyrh9</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>19dyhyg</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>Am I doing something wrong?</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqlss8bv49ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>19dyhb2</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>OPI - Show Us Your Tips!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dyhb2</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>19dyeyv</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Looking for Opinions: Beaux Reves, Phoenix &amp; Nailed it (formulas)</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dyeyv/looking_for_opinions_beaux_reves_phoenix_nailed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>19dyau4</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>Not even 18 hours since finishing the painstaking cat-eye process 😭🫠</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yo55gla539ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>19dxyfg</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t>Stamping fun with Fairy Dust ✨</t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dxyfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>19dxvmo</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Obsessed with Venetian Sky</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/osfcgmtc09ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>19dxow6</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>Sheer/semi-sheer polishes with vibrant shimmers?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayeijg1xy8ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>19dx3d7</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>I broke (a)nother nail 🥲</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/bLrdnZy</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>19dwd5v</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t>Help me decide!</t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dwd5v</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>19dwcg0</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Down for brown 😀</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/4cUXy8F</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>19dw9dx</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>How often do you change up your mani?</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dw9dx/how_often_do_you_change_up_your_mani/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>19dw61e</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t>Builder gel</t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dw61e/builder_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>19dw4al</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Nail extensions with hema allergy?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dw4al/nail_extensions_with_hema_allergy/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>19dw19w</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Velvet effect not lasting</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dw19w/velvet_effect_not_lasting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>19dw0a2</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Valentine’s Day Mani (glitter jelly and silver)</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dw0a2</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>19dvvcs</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Remainder: polish is not edible</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dvvcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>19duxt3</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>First Cuticula polishes for me - Kraken’s Wrath and Twilight Dragon</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19duxt3</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>19du66l</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Such a Farse and Black the Night</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19du66l</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>19du4fr</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Dupe Request for Color Club's Hello Holo</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19du4fr</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>19dtthn</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Unintentionally got a really cute color</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39w03s2r68ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>19dswpl</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Why does my polish chip off after only a few days?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dswpl/why_does_my_polish_chip_off_after_only_a_few_days/</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>19dswbl</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>accidentally over filed my nails, need advice</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dswbl</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>19dsqx1</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>Why do my thumbnails always break in the same place?</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19dsqx1/why_do_my_thumbnails_always_break_in_the_same/</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>19drtz9</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Advise for a newbie</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19drtz9/advise_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>19drkto</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>ILNP</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6nia6nep7ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>19dqv5h</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Daughter's Curated Collection</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yeqb99luj7ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>19dqh2i</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>A mani to match my favorite jewelry</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2zuqc3ng7ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>19dqgpd</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>Mooncat Mortals Be Warned</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dqgpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>19dp77n</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Stamping resizer</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dp77n</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>19doxho</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Identifying Thermals</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19doxho/identifying_thermals/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>19dnxqk</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>ILNP - Pool Party w/ Matte TC</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dnxqk</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>19dnanw</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>A couple years ago my mental health was in the toilet, so I put how I REALLY felt on my nails 😂</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dnanw</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>19dn6zb</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Did winter nail art on my friend’s nails!</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dn6zb</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>19dlx0n</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>Emily de Molly - Holding onto Hope</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ab63ioio86ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>19e9qda</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>my very first time trying nail art 💌</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e9qda</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>19e88vj</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t>some of my favorites designs of the last year</t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e88vj</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>19e79l2</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I love my new 3D Gel Set!! My nail artist always makes the most special designs turn out perfect 🥹✔️💅🏼 ( ChiChi nails in Ontario ) ( cuticles are fine camera turns them a tinge red but they’re perfect )</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gx31jdxz2bec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>19e6zpe</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Nightmare before Christmas Wip</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hlellsll0bec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>19e6lrr</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t>cherry bomb set by me🍒🖤</t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e6lrr</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>19e4w7c</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t>Pink chromey sky with Cupid 💖</t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19e4w7c</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>19e3vll</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t>Pink Hearts</t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y4602sdy9aec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>19e39m4</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>Porcelain</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/848s50uw4aec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>19e1jfe</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hot pink and black gel nails </t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8lucivvbr9ec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>19dzpgt</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t>Little tomatoes 🍅</t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lzzy6jdtd9ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>19dwh79</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>Some nails I did in 2023. Some worse than others , but I’m excited to improve more in 2024! Would love to get better with nail art.</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dwh79</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>19dvozc</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>Got a ways to go, but slowly getting the hang of it</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dvozc</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>19dtcdj</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>XOXO Love Nails - took the length way down</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19dtcdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>19do51p</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t>🫶🏻</t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ol9mv6ucw6ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>19dn94d</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>My nail art work on natural nails.</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s22vkexjn6ec1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 25 08:08:19 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C606"/>
+  <dimension ref="A1:C760"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10735,6 +10735,2624 @@
         </is>
       </c>
     </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>19f45mb</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Two months of growth and they are intact 💅🏼✨</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2um4egl1kjec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>19f3uoi</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>Flowers and stuff</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nbskuvpagjec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>19f3bgm</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t>(chichi nails in ontario) I’m absolutely obsessed with 3D Art😩💅🏼🤩</t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2on2e27t9jec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>19f2dzc</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>Vaca nails help</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f2dzc</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>19f1sls</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Single's Valentine nails</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f1sls/singles_valentine_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>19f1ldi</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>Why won't my nails stay???</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f1ldi/why_wont_my_nails_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>19f1dbz</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Non-gel alternative to builder?</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f1dbz/nongel_alternative_to_builder/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>19f172s</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>I love this shape it's one of my favourites❤️</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7ovi5qyeniec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>19f0vxe</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>Watercolor nails</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f0vxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>19f0gjs</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t>Sns vs tips</t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f0gjs/sns_vs_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>19f0cyy</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>New nails - What do you think?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hoxxuke8fiec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>19ezr49</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Advice?</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/chjlv4sj9iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>19ezn7c</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t>Matched my mug</t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/715dkkpi8iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>19ezmqf</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Is there anything i can do to save the length? Or is the nail too cracked to salvage?</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lkgtqq4e8iec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>19ezcd0</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>More sets from the spicy days!</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ezcd0</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>19ezbmr</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>Do you think my nails should be longer &amp; I should try red next time?</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4gknqell5iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>19eyrxa</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Need your help!!!!!!</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eyrxa</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>19eyonm</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Why do they look like this? Green Flash</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6vxp7n5yzhec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>19ey3ed</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>loving them 😮‍💨😮‍💨</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3i8nqg6luhec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>19exrfi</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>I now keep it simple. But I use go hard on the nails…. Swipe! Is it cause I’m older now?</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19exrfi</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>19ewya6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>I’m concerned about the spike in gel allergies</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ewya6/im_concerned_about_the_spike_in_gel_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>19evy5n</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>Trying different shapes</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19evy5n</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>19ex0bv</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Monomer and Acrylic Issue.</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ex0bv/monomer_and_acrylic_issue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>19ewzhn</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>Thoughts on shape?</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ewzhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>19ewvlz</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>french tips done on my natural nails :)</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ewvlz</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>19ewpye</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Love how wine-y the color of my nails look like under the sun.</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8kyak5fmihec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>19ew302</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>opinions prt 2</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g5ictlfkdhec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>19ew2l4</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>opinions?</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ew2l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>19ew05b</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>KISS nail kit UV lamp</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wzbdyqzwchec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>19evzyg</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Yasssss</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/08prw88vchec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>19evrvn</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>My nail is lifting and i need advice</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3jbr40a1bhec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>19etjy1</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>Red French manicure</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19etjy1/red_french_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>19ev9dt</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>valentines 💘</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2lgq1gxz6hec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>19ev3lh</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>Existential Crisis ✨</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ibgspoer5hec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>19ev03z</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t>Might be my favorite set</t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ev03z</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>19euaau</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Does square fit my hands?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2vxh9ooizgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>19eu4ki</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>winter bunny nails 🐰</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xtrxvtbbygec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>19ett9y</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>Valentine Nails ♥️</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oa4nq2k0wgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>19eswd4</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Valentine's Day Set</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eswd4</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>19esw9t</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>How is this apex? I'm still figuring out polygel</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpzwy1k7pgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>19es3m0</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails by me!🌹💖</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19es3m0</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>19erzsl</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>First time trying any matte colors</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19erzsl</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>19eqepm</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>How do I stop this from happening?</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qqcyw717gec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>19erv42</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Love the design but I might hate the set (on me atleast) ???</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jv79hhuohgec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>19erl5k</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>What color nail polish should I get with this dress ?!</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vouywnmfgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>19erjst</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>🏳️‍🌈</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/so5807tcfgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>19eqo14</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>This glitter just wont quit.</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eqo14</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>19eq9ju</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Found my new nail tech!!! 🥰 Sweet &amp; Simple Valentine nails 💅🏻💖</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eq9ju</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>19eptwd</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Is it too early for valentines nails?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eptwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>19epojk</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>First time using gel nail extensions!</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c1f13rs1gec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>19ep62k</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t>Are these nails worth getting a touch up for?</t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ep62k</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>19eoxh6</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Cute nails</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hkx9tlgdwfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>19eou1a</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Jumping in on the nude trend I’m seeing today.</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sr966cmovfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>19eokv6</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Why does this keep happening?</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cq9xznlutfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>19eobt7</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>Feeling wintery</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0f32y1l0sfec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>19enpyd</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Why does my rubber base keep popping off</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19enpyd/why_does_my_rubber_base_keep_popping_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>19elcwd</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>Nails destroyed after shellac removal…normal?</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19elcwd/nails_destroyed_after_shellac_removalnormal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>19ent0i</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>Just some natural nails for a change</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p8legozeofec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>19enhir</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>Do you still remember tamagotchi? ʚ(* ´꒳` *)ɞ 💗✨ I still play mine!~</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19enhir</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>19enc0e</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t>She's sitting all pretty 10/10😍</t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ojcion4lfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>19en1n9</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Nude Almond</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19en1n9</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>19ejc3v</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>What to do about crack in dip and natural nail?</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ry4xy85nmeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>19emcgo</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>Proud of my self for these</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19emcgo</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>19embkd</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>Sparkles are my go to</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m1fy10399fec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>19em1me</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t>What is your go to base coat and top coat? I'll go first</t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfgg2kb97fec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>19eldnd</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lbgu9nna2fec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>19el9nv</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Nail shape suggestion</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/csmz96ah1fec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>19ekol5</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Does anyone know of a good dupe for NARS Zulu ?</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ekol5/does_anyone_know_of_a_good_dupe_for_nars_zulu/</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>19ekjfy</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>Chrome Valentine with a hidden surprise</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ekjfy</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>19ekgd5</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t>Bday mani!</t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w62of6m9veec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>19ejy8i</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>How do I use Nail Repair Polish?</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ejy8i/how_do_i_use_nail_repair_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>19ejugc</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>New nail tech</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ejugc</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>19ejgvd</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>🔥</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fm6l17cpneec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>19ejc86</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>valentines nails 🤍</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lh70jnaomeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>19ej7ws</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t>Are you a press on or acrylic girly?</t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19ej7ws/are_you_a_press_on_or_acrylic_girly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>19eil3v</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>valentine’s day natural nails</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bozw855mgeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>19ei16j</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t>My first French manicure was done on someone</t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/spv54dl1ceec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>19ehzda</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>First time doing square sets. Really disliked them at first buuut they eventually grew on me 💖</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ehzda</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>19ehxrq</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>hello kitty french tips</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ho0z498beec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>19ehp5x</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Spring in Winter</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ehp5x</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>19ehe73</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Fresh year, fresh set</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gxgj5cxm6eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>19eh17l</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>I have been pretty much neglecting my self care since my kiddo was born 3 years ago. I decided to start getting my nails done again. My journey so far. 🥰</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eh17l</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>19egzrs</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t>Back to red ♥️</t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qjy0molz2eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>19egw8j</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t>Tried red nails for the first time ❤️ Love them</t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nh9cpez32eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>19egvq9</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>Biab growth</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eukrwhty1eec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>19egt0g</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Classic French tips with a little something :)</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x84ltht71eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>19egokn</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>2 hours well spent with this kuromi sets</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/36ct36s30eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>19egmx3</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>I stopped cutting my cuticles and started using cuticle oil</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/efch2yeozdec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>19efz9a</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>DIY Valentines Nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w13sx799tdec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>19efprz</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>Just started to do my own nails recently...What do you think of this?</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19efprz/just_started_to_do_my_own_nails_recentlywhat_do/</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>19efiw8</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t>my go to custom nude mix ❤️❤️</t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19efiw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>19efhj0</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>junk nails!</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19efhj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>19ef8i4</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>French but in different style! 🥰</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ef8i4</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>19ee9yr</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>First time practicing with magnetic “cat eye” polish on natural nails~</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qllylwhgadec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>19edd2b</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>New set 🍒🍩🥰</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19edd2b</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>19edfzg</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>Aurora nail / ice nail salons london</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19edfzg/aurora_nail_ice_nail_salons_london/</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>19ecfcv</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t>Moulin Rouge nails 💕</t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ecfcv</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>19f3asm</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t>Essie tiers of joy dupe?</t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x33elk6l9jec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>19f25l8</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>Started walking every day on an incline since Sept--lose 30 lbs AND stopped biting my nails entirely!</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hhpdlg1wwiec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>19f1qy1</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>Finally done!</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rgr8t8yxsiec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>19f0oxl</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>Woke up and chose prugly 🫠</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f0oxl</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>19ezp3y</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t>Deceptive lighting</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os80n3919iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>19ezk8g</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>So happy with my valentines nails!</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1w4vno4r7iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>19eyx31</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>Nail tech is exhausting 😔</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19eyx31/nail_tech_is_exhausting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>19eyvm3</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>Finally swatched and labelled my whole collection (to date)</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zqlo4jho1iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>19exyu1</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Highly recommend matching your nails to your ring</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/14kr4rflthec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>19exlpq</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19exlpq/help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>19ex30q</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Does anyone else take nail pictures on the subway? 😅</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ex30q</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>19ewgf9</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t>Vampy Red</t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ewgf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>19ew43h</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>[Magnetic] Experimenting with magnets and polish, got this awesome cross/star pattern!!</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dct1gl7idhec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>19ew1em</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t>A Winking Light by Polished for Days</t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/v6tp50d7dhec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>19ew0n7</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>ILNP Pixie Party 🧚🏻‍♀️✨💕 Please recommend any other polishes with this kind of sheer, sparkly, shifty magical formula! 🙏🏻</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ew0n7</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>19evtlf</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Don’t let anyone tell you your polishes are too similar; make a skittle out of it for a subtle mix up look :)</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19evtlf</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>19evh42</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>It’s giving…burnt cheese</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19evh42</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>19ev1hk</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t>Latte Cloud vs Silken Path vs Does It Get Eddie Vedder</t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ev1hk</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>19ev1bm</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>Existential Crisis ✨</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3bv5mhj95hec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>19euion</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>My nails remind me of watermelons 🍉</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u9hklqob1hec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>19eudmk</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t>ILNP Jackpot 🖤🌟🖤</t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7mchvd550hec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>19eu3mg</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t>sparkling water ✨</t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5rove054ygec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>19esld9</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>Seche is so glassy! First mani of 2024</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xhu8xnh1ngec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>19es983</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t>I couldn’t find any pics of this online, so here’s Pop Arazzi “Calm Winter”. Cvs brand Mystic Moonstone dupe?</t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19es983</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>19es3he</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>My first time giving myself a manicure!</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pt7gbpedjgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>19erem7</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Basic milky nails</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc4wuhvaegec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>19ert0p</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t>Haven’t done creams in a while… and I miss the sparkles!</t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ert0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>19er9vh</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Bury me in sheer glowy goodness</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mirzrwi0dgec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>19eqz2v</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Death Valley Nails</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19eqz2v/death_valley_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>19eq04b</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>How do you make polish smooth and hide peeling or other marks on nails?</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8pvitly24gec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>19epu2w</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t>Help with replacement brushes</t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19epu2w/help_with_replacement_brushes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>19ep1mk</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>So Cold, Brr by Shleee Polish</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xid7n67xfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>19eofjy</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t>Someone commented with an alternative velvet hack, and I tried it!</t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/comdzz7rsfec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>19eo9k9</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t>Feeling wintery</t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3mm4q11krfec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>19eo6wo</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t>Is something happening at Color Club?</t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19eo6wo/is_something_happening_at_color_club/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>19engo6</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Mooncat Head in the Clouds</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19engo6</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>19enedq</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t>Favorite polish with strong color shift?</t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zourtjlllfec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>19enen7</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>BRIGHTEST, most neon pink polish you've found?</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enhqys5nlfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>19en7sj</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>First time with Covid, stuck at home and unable to show off this whimsical beauty of a polish. Thought you all might appreciate it!</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2zc4kpdckfec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>19em3ik</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t>What are your go to base and top coats? I'll start:</t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/00nw9vkm7fec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>19elkoa</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Best self-mani of my life</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19elkoa</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>19ekggj</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Lake of the Clouds ☁️</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ekggj</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>19ek1st</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Bright and Polished</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19ek1st/bright_and_polished/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>19eju6w</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Death Valley Om + Dill Weed + Matte top coat</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g4g0x98kqeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>19ejoby</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>Retiring DVN shades!</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8tz4o3rbpeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>19eji9x</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Cirque Colors Aqua Jelly and Spotted</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mxtpjdvzneec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>19ej8lt</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>First order from Mooncat! I couldn’t decide which one(s) to paint with so I chose all.</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ej8lt</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>19eh914</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t>Early birthday nails</t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hld4is2a5eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>19eguts</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Spring Green Skittle! 🌱</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19eguts</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>19f4byj</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>(chichi nails in ontario) I’m absolutely obsessed with 3D Art😩💅🏼🤩</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z35ie05bmjec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>19ew9lq</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>Abstract Pastels and Gold Foil</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pss59ql4fhec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>19evrun</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>designs for older women?</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/19evrun/designs_for_older_women/</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>19eonnw</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>spring mood 💅🏻🌸</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ygx1rupeufec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>19eolx0</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>🤭It's very cute, isn't it?</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7kyk1c2ufec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>19ejqvv</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t>Go Lions!</t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yds6jx7vpeec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>19ehaej</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>🔥</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qi4t6fzo5eec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>19ef99i</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>2 different French 🥰</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ef99i</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 26 08:07:40 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C760"/>
+  <dimension ref="A1:C954"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -13353,6 +13353,3304 @@
         </is>
       </c>
     </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1abdcp8</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Beetles 'Nail Strengthener/Hardener' Gel?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abdcp8/beetles_nail_strengthenerhardener_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>19fnjhz</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>Now a press on girlie</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fnjhz</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1ab5yg1</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>Having so much fun applying press-ons. Swipe for my process. Y’all were so kind on my last post here it’s inspired me to continue this act of self care 💜</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab5yg1</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1ab9dqw</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t>Porcelain inspired nail design</t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wl5zank5lpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1abbr3x</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>Question for a Newbie</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abbr3x/question_for_a_newbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1abbnae</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>I’m obsessed with these.</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b981jr0q7qec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1abblnr</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>I decided to give up the long nails and went back to shorter and classier</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abblnr</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1abbcuq</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t>Gel polish first go!</t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wn7knytq4qec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1abakw9</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t>I need some ideas for my nails for Feb. I’m not even sure what I want. But not red or black. I would prefer short nails but I do get acrylic nails.</t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abakw9/i_need_some_ideas_for_my_nails_for_feb_im_not/</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1abad0y</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>My nails might be a little too wide for this shape 😂😂 and my fingers</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abad0y</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1aba693</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>LOOK AT MY FIRST NAIL GEL EXTENSION!! 🤩</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4dl7v62rspec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1ab9jcp</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t>Happy Early February</t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/70vi1irlmpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1ab8w8z</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t>What do you think?</t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab8w8z</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1ab8q0a</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Nail progress!</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zd1jhc31fpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1ab8ikk</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t>second set of mardi gras nails 💜💚💛</t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxp63lx5dpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1ab8b8u</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>Start a nail tech course Monday, here's my final set before I've got to remove my claws for a bit! Temp sensitive gel over some holo sparkles</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/un6o5x5fbpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1ab83kv</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t>First time using gel polish over my polygel extensions</t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jb2n05bl9pec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1ab82l3</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>How to keep nails from Chipping?</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ab82l3/how_to_keep_nails_from_chipping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1ab7ud7</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Valentine's set one</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab7ud7</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1ab6zas</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t>Vday Cat Eye 💅🏼</t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jo5bdewzoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1ab6o2x</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Haven't had simple nails for so long.</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ab6o2x/havent_had_simple_nails_for_so_long/</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1ab6kg6</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>First time doing a solid color in over a year!</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2z9ha0bdwoec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1ab69hw</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Best natural pink DND gel colors?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ab69hw/best_natural_pink_dnd_gel_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1ab67uz</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>Finally did my own nails</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab67uz</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1ab65fk</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>Removing sticky layer without alcohol?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ab65fk/removing_sticky_layer_without_alcohol/</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1ab5p97</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t>My nail tech did an amazing job with these black lace acrylics!</t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ykgt3cr2poec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1ab5o4k</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>new valentines nails 💓</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5ppouwxtooec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1ab59sq</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t>Longest I’ve been able to grow my nails out to!</t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab59sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1ab56eq</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Critiques?</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab56eq</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>19fnwy8</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t>Am i getting scammed</t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dsmpcnzoeoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>19fnvn1</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>V-Day mani</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t877er6eeoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>19fntj6</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>My gorgeous set (Cincinnati area)</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mcfgcs7xdoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>19fnlzt</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>Ready for Sunday🔥💙🦁🏈</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gg3wc3u8coec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>19fne0x</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>I love the glitter claws</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rga96n1haoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>19fn584</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>I Call These 'Four Hours Later' 🥹</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s6syq4oh8oec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>19fn2at</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t>Sometimes my Dollar Tree gets name brand polishes packaged for dollar stores. Got lucky and had a major Revlon haul tonight. They had others too but they were ones I already had in my collection.</t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fn2at</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>19fmxph</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>Uñas Naturales en proceso de recuperación aplicando aceite todos los días</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ivw5jrit6oec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>19fm4nb</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>Chrome</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2ogntkf0oec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>19flu9u</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t>honest opinions?</t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19flu9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>19flrq9</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Natural Ora Set done by my nail tech. Acrylic on my natural nails.</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ibobv4nxnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>19flf9l</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Sweet dreams set</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19flf9l</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>19flcwj</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t>First "Nail Design"</t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8st595bjunec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>19flazl</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>First time getting french tips!</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rf4kwxc5unec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>19fl68i</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>HELP!! What shape fake nails should I get?! Should I get acrylic, dip or gel?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fl68i</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>19fl5r4</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Those who go to the salon: Does yours have listed prices? Would it be a red flag if they didn’t?</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fl5r4/those_who_go_to_the_salon_does_yours_have_listed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>19fkym7</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Baby Girl Aura nails 💖</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fkym7</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>19fkqn6</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>Nail tips</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fkqn6/nail_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>19fk7dn</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>Worth getting a manicure or no?</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fk7dn</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>19fjzem</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>New acrylic set 💅🏻</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/enmn4io9jnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>19fjfi9</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Happy Valentines</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x8mfqj15fnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>19fj9sd</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>I did my friends nails. Went for an abstract look</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fj9sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>19fiu4c</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>One day I won’t have Frenchies 💅</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fiu4c</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>19fipmu</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Would you ask them to re-draw this design?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3hc38jpr9nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>19fikve</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Had to cut my nails short because they break easily. 🙄Tried a new color today: lady green. I love it!</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5ar3tgs8nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>19fi2xu</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>Just got polygel for the first time!</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fi2xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>19fi0go</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Did my own nails with a gel nail kit - how did I do?</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jmntsh5l4nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>19fhxh1</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Purple!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fhxh1/purple/</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>19fhtp5</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>*sigh* The struggle as a working man is real. Wish i could get more than 24hrs out of a set.</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/odjrlxb43nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>19fhqgy</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Finding Good Quality Press Ons</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fhqgy/finding_good_quality_press_ons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>19fhnjp</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Make it a grown-up-goth French for me!</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/299dks9t1nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>19fhjhn</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>My nails are natural and they need a change! what color do you think will look best on me?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uguhnepy0nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>19fhh5x</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t>Shape isn’t perfect, but I’m proud of these 🥰</t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zx46zk1f0nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>19fhf0e</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t>Do you like this nail design?</t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x5hc0p210nec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>19fhc6t</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Can I use a UV base coat with regular polish?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fhc6t/can_i_use_a_uv_base_coat_with_regular_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>19fh0o0</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>bday nails 🎀💕</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fh0o0</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>19fgy33</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>I wasn’t able to get nail extensions for a whole year because of my job. I recently quit that job so I decided to treat myself :)</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dhsb43riwmec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>19fgwim</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This week office nails </t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/vhkgs7o6wmec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>19fghbg</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Frenchies are my favorite</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fghbg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>19ffzu3</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>What are these, where can I buy these?</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8wwumeu9pmec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>19ffwle</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>How to say I’m a 90s kid without saying I’m a 90s kid</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c5p3fobjomec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>19fffw7</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>Love is in the air 💕</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fffw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>19ff7i1</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t>Cre8tion soak off mermaid gel - Colour 33</t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/567sd7aejmec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>19ff1pd</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t>I love all the flake colors in this dip!</t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ff1pd</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>19fepmb</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>Prep advice needed! :-(</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fepmb/prep_advice_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>19fe596</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>My first sets</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fe596</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>19fdxsg</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Press-on or night before?</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fdxsg/presson_or_night_before/</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>19fe1yn</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t>I’ve always been insecure about the white stuff around my nails on my skin, I have no idea how to treat it and make my nails look pretty. I want to keep up with them myself but have no idea how to, please help💗</t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fe1yn</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>19f33rz</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Best nail whitener or other advice</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f33rz/best_nail_whitener_or_other_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>19ez6hr</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>First Time Trying Black Polish</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9fpw45fe4iec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>19eypus</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Nail tech is exhausting 😔</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19eypus/nail_tech_is_exhausting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>19fdf8h</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t>Dark nails are so pretty 💅</t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/amw3d7f76mec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>19fd2bb</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>Four nails curve downwards -- what to do?</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fd2bb</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>19fcybk</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>first attempt at acrylic nails</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fcybk</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>19fcvur</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>Testing out my new nail stickers (2 diff lighting) 💅</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fcvur</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>19fclw1</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>First time with green tips</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r76e6gvvzlec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>19fcall</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t>Embracing the natural look</t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h56g5midxlec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>19fbyub</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5kp5qtmqulec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>19fbyew</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Early Valentine’s Day Nails!</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fbyew</t>
+        </is>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>19fbhhb</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>nail designs so far 🫶🏻 should i do purple, blue, or orange next time?</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fbhhb</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>19fa6sl</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Press on collection</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19fa6sl/press_on_collection/</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>19f9rnt</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Made my nails today but not sure whether the job was done right or not</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/atkdz6ghclec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>19f9pe7</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>New Set 💅</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f9pe7</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>19f9njm</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>These need to be fixed right?</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f9njm</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>19f90ag</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - Baby Billy's Bible Bonkers</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f90ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>19f8s8d</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>Lilac tenderness</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yul2zfqr3lec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>19f8rch</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>can builder gel be ‘heavy’ on natural nails?</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f8rch/can_builder_gel_be_heavy_on_natural_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>19f85ah</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>First Chrome Set!</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ouqc5v8exkec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>19f7l5o</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Is it pink or is it lilac? Either way I’m loving it!</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f7l5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>19f5zxt</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>How can I make my dip nails look shiny again?</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/19f5zxt/how_can_i_make_my_dip_nails_look_shiny_again/</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>19f5np4</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t>Finally managed to get a new manicure after my previous set survived a missile attack (with two broken nails)</t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f5np4</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1abd86m</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>Orly Bonder vs Glisten &amp; Glow Sticky</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abd86m/orly_bonder_vs_glisten_glow_sticky/</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1abcbkd</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t>Any idea why this is happening?</t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abcbkd</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1abc9w7</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t>Blue skies and calm waters</t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abc9w7</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1abbmfx</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t>Which color should I adopt as signature nail color?</t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abbmfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1abb2db</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t>I bought this polish just bc I liked the name</t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5wonn5wo1qec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1abahwk</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t>Please tell me what I’m doing wrong!</t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abahwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1ab9bzm</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>🍒🍇</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6va9sd6okpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1ab809g</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>Healthcare workers, how do you protect your cuticles when washing hands is required all the time?</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ab809g/healthcare_workers_how_do_you_protect_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1ab7vcd</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>It’s always so hard to do the second hand evenly, but I’m pretty proud of these.</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3ppvav3l7pec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1ab7b56</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Nails In Spaaaaace!</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab7b56</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1ab75w7</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Thoughts? Comments? Gripes?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lahe6lpf1pec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1ab6sa7</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t>This polish is so beautiful but…</t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bxv5x6m8yoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1ab6723</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>ORLY Ripple Effect (Aqua Aura Color Pass!)</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hczvxls3toec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1ab66q5</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>Zoya - Aurora</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ox9q5dgusoec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1ab66rg</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>Bubbles in my top coat?</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ab66rg/bubbles_in_my_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1ab5zdq</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t>New love</t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/osh818tbroec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1ab5shr</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t>Why doesn’t my gel last?</t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ab5shr</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1ab5c76</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t>Mishipeshu (The Great Lynx)</t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w6daroehmoec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>19fnxnj</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>My neon pink mani (already) Thank you guys for the polish recs!!</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fnxnj</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>19fnplv</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>Gel polish</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fnplv/gel_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>19fnk27</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>Allergic to nail glue, but I love press-ons - any adhesive alternatives?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fnk27/allergic_to_nail_glue_but_i_love_pressons_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>19fnism</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>Thin/Breaking Nail Advice</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fnism/thinbreaking_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>19fnft5</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Please help me pick my manicure, I’m overwhelmed 😢</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fnft5/please_help_me_pick_my_manicure_im_overwhelmed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>19fndvh</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>my first go at nail art!!!</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fndvh</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>19fn4n0</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t>Like a beautiful tropical fish</t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y0pxay0d8oec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>19fmrqg</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>This might be one of my favorite shades I’ve ever tried.</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/74k8pb1i5oec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>19fm6l4</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t>I don’t normally go for darker polishes but I love this shade 😍</t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fm6l4</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>19fm0ty</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>what’s yall favorite hand position for nail pics 😻</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fm0ty</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>19flf9v</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>Love when you find random lighting in public that make your nails pop ✨</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19flf9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>19flcpw</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>First post here! First time getting french tips!</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4etgntzhunec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>19fl60t</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>To trim or not to trim?</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fl60t</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>19fkyae</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t>The reason why I don’t bother with magnetics 😭</t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fkyae</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>19fkvei</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>no sun in sight but this baby still glows! ✨💙</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e8rddm9sqnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>19fk8gj</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>For when your heart is dark but also shiny</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3g9j6yr4lnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>19fk4tv</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>Rhinestones</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fk4tv/rhinestones/</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>19fk4hq</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>V-Day Mani</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cs2hreqbknec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>19fjzdn</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Reminds me of those shiny beetles 🪲</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i5ijm4g9jnec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>19fj3fq</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t>Polish Request - Nails the Color of Heartache</t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fj3fq/polish_request_nails_the_color_of_heartache/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>19fi3sd</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>The Power of Undies</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fi3sd</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>19fhw42</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Natural nails keeps breaking or being uneven, any guide on how to have an overlay+ classic polish on top? I’m a complete noob!</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fhw42/natural_nails_keeps_breaking_or_being_uneven_any/</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>19fhj6x</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Shape isn’t perfect, but I’m proud of these 🥰</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cl1ushcv0nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>19fhc7c</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>Challenge nail</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fhc7c/challenge_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>19fgwff</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t>Update: arranged my swatches in rainbow order</t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fgwff</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>19fglqa</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>Help (in description)</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fglqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>19fg2vq</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Why print a magnet holder when you can have a little guy help you out!</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/co134muxpmec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>19fg0hc</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Red glitter jelly</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/vXlJJPM</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>19fft23</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t>Do reflective glitter polish tend to be more goopy?</t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0ob8wcmtnmec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>19ffisr</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>Dupe for Ciaté Apple &amp; Custard</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19ffisr</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>19ff5cu</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t>Dental retainers and long nails</t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19ff5cu/dental_retainers_and_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>19ff2u6</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Rave for Wet n Wild Topcoat</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jkzj8g9fimec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>19fdg4f</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Tasha 🤎</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fdg4f</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>19fdg12</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>China glaze fairy dust?</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fdg12/china_glaze_fairy_dust/</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>19fda90</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t>So ethereal 🧚🌟</t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6ic1jxe65mec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>19fd6e0</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Best Essie &amp; OPI base coat and top coat?</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19fd6e0/best_essie_opi_base_coat_and_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>19fcat8</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>never posted my celebratory nails!</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fcat8</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>19fbwws</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t>Magnetic paw prints!</t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/C2U2JKTska7/?igsh=MW9nYno5ZnZnOWFpeg==</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>19fbjod</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>neon rainbow skittle 🌈</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fbjod</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>19fbf79</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t>I'm devastated</t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fbf79</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>19fb36o</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>The BEST velvet nails I’ve ever done (and easiest)!</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4wxum90onlec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>19fappp</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>Experiment with fidget textures.</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/656cjq7nklec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>19fanoz</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Soooo no one could decide on a shade of pink, so I did all of them</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1hg43rg6klec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>19f9xqa</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>Classic black and white</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f9xqa</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>19f9cea</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>My fingernail polish takes over 24hrs to dry</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19f9cea/my_fingernail_polish_takes_over_24hrs_to_dry/</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>19f95zn</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Swamp Gloss - Baby Billy's Bible Bonkers</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f95zn</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>19f684p</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t>Vibrant Scents F&amp;H vs Glisten &amp; Glow TC</t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/19f684p/vibrant_scents_fh_vs_glisten_glow_tc/</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>19f5lse</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>My new favourite gel polish</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f5lse</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>19f4m3j</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>This shade is so pleasing 🩷</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1fs0lrnupjec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1abb0j1</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t>Sea Shell press on nails 🐚</t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abb0j1</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1aba6a7</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t>Purple Marble Nails</t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aba6a7</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1aba5am</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Pride nails</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pyy1k0whspec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1ab8v2a</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t>Porcelain inspired nail design</t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yxig0f5agpec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1ab6wo0</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a care bear set 🎇 tutorial on my tiktok ☺️ can't wait to finish </t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/fj609vn9zoec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1ab683k</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Hello Kitty Inspired V Day Set</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g2qqoradtoec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1ab5yjy</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>kapping in acrylic, I made this design with gradient on the petals, using half the brush of one color and half of another color, I make these designs freehand</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/skdq09w4roec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>19fnt1k</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I’ve been into dimensional/treasure box nails lately—Thoughts? </t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/g65oi06sdoec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>19fne18</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Sets from this week ✨</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fne18</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>19fm4pr</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Amazing inspo</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fm4pr</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>19fm0v0</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Some V-Day inspo from @sinvnails</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ue1jqhklznec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>19flgo4</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>Studio ghibli nail set I made</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19flgo4</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>19flcr6</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>Sweat dreams set</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19flcr6</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>19fkvpf</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Baby Girl Aura nails 💖</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fkvpf</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>19fk1rv</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t>It’s never too early for VDay mani’s.</t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h95o44tqjnec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>19fhlo7</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>Make it a grown-up-goth French for me!</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u7hi8vxe1nec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>19fg58n</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>Roses and crystals and snow</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mfdkpc97qmec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>19ff4u6</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>Monopoly nails by @nailzdesignzc on IG</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/woi1dp2vimec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>19feryq</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Drawn using only a dotting tool with cheap wet n wild polish and a nude rubber base</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iwmeoiuzemec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>19fbzk9</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19fbzk9</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>19fbgzr</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Could we please ban AI "art" from this sub?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/19fbgzr/could_we_please_ban_ai_art_from_this_sub/</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>19f9qgd</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Something fun to beat the winter blues 💅</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f9qgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>19f8thd</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>New to Nail Art :)</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/05ffq4e14lec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>19f8md1</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>HI BARBIE, HI KEN 🎀🎀</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tohnd5862lec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>19f6o8d</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/19f6o8d</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>19f5st4</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>Realistic 3D spider nail art made with sculpture gel!</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j8wngsib5kec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>19adwt9</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Want to see your Valentine's Day nails😊😊</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/19adwt9/want_to_see_your_valentines_day_nails/</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 27 08:07:10 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C954"/>
+  <dimension ref="A1:C1149"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16651,6 +16651,3321 @@
         </is>
       </c>
     </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1ac45o7</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Fresh set</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wjnow3zbcxec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1ac3q1b</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t>Sailor moon inspired nails</t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gciuhneq7xec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1ac3ua4</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Can you get acrylics done on bendy fragile nails? Does it help strengthen them?</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ac3ua4/can_you_get_acrylics_done_on_bendy_fragile_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1ac2mhb</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>2nd air brush set!</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdynse9twwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1ac25xx</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t>Lavender Nail Polishes</t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ac25xx/lavender_nail_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1ac21ts</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>valentine’s day nails 🩷</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vxuz0s5rwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1abxyyq</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>Flash Cure Lamp Recommendations</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/diidf1xgqvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1ac1p4q</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t>DIY Valentine’s Day Nails</t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac1p4q</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1ac1ln0</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Progress pic!</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu7d286xmwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1ac1g72</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Were these worth it</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac1g72</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1ac1fqr</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t>It’s almost been two weeks - should I get them redone tomm or wait for Tuesday?</t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgmrkfgelwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1ac16xn</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Tried painting rain drops on my daughters nails the other night</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac16xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1ac16bn</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t>Just starting out, any tips for beginners?</t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qtwt845yiwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1ac11kr</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Mixing some Kiss USA press on packs. These’ve lasted a whole week and still going strong!</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sx9ikfjphwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1ac0j8x</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>i want to try poly gel. where do i start?</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ac0j8x/i_want_to_try_poly_gel_where_do_i_start/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1ac0j6s</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Old lady new nails</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p07eou11dwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1ac0f2u</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>Blue &amp; Pink</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0f2u</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1ac0aff</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>Press On Nails, just finished. What do you think?</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29qi2zpsawec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1ac09nz</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Nails bending</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac09nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1ac01g2</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>3d snake :3</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac01g2</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1abzkmu</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Have you recreated designs from girls in the community?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abzkmu/have_you_recreated_designs_from_girls_in_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1abz85n</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abz85n</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1abz6y6</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>Nail art!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abz6y6</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1abyk0j</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>Reputation nails 🖤🐍</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m42zzjdvvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1abybwy</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t>What nail shape would you recommend?</t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kam3ec9gtvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1abxx6w</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>🍄 nails!</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abxx6w</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1abxwgj</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>What works best for natural nails that won’t destroy them afterwards?</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abxwgj/what_works_best_for_natural_nails_that_wont/</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1abwszi</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>Do you like nails with rhinestones?</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/479ck76ygvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1abwfgc</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>First time with poly-gel. Not perfect, but I think it's pretty cool (pun intended)</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o15dzntxdvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1abvyzm</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Looked</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iqnju96cavec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1abvkmf</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Today’s strawberry bubblegum🍓</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mrbdko97vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1abva2z</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Early Valentine’s nails :)</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6loeyxv05vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1abv7mu</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t>Just got my nails done earlier today, do they look good? 🌟 💙</t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/da1ezoxi4vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1abuxyr</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>just got my order, help me choose !?</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dkcjd8ah2vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1abuj9a</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Being a DIY girlie needs a whole new level of patience</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abuj9a/being_a_diy_girlie_needs_a_whole_new_level_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1abtpww</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t>Always been a nail biter due to anxiety, I have a wedding coming up and I wanna fix it ALL</t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5lf9vcw8tuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1abv2ew</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>My natural coquette nails🎀❤️</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n6s5lcaf3vec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1abv19d</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>Help! I can’t keep gel on my index nails.</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abv19d</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1absrg8</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Nail polish help!</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1absrg8/nail_polish_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1abuzej</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>long almond acrylics</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/85e5vswr2vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1abuwzs</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Night sky 🌌 ✨</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/os3sav1a2vec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1abuhim</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>cute &amp; simple valentines set on a client :) I love my job</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x11avtwwyuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1abuf97</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t>New polish</t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abuf97</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1abu2ng</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>Mani and pedi ready to go back to lecturing 💅🏻👩🏻‍🏫</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abu2ng</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1abtzru</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>Valentine’s set by me 🎀 still improving!</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fq5tfxhdvuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1abtbp4</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t>tragedy almost struck 🥺 shout out to the teabag method ✨✨</t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abtbp4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1absiu3</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t>Fucked up gel removal</t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7b5koe99kuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1abs9nz</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>Birthday set!</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xn25go9biuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1abs8cl</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>First time doing my own gels for years. It shows.</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4ddfedo1iuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1abq44p</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Mystery Machine Inspired Gel Nails</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abq44p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1abr648</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>will get as many aesthetic photos of my nails as much as I can before I need to get a full !! ( candy cream matte finished look ) done in Ontario at Chichi nails salon 🍭</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e81w7532auec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1abr4f6</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Which shape suits me better</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abr4f6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1abqyze</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>Slytherin nails!</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/65oxezsh8uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1abqpu1</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>How did I do?</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtgz2k7k6uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1abqfbe</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Happy with this purple set 💜</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jnoepvjd4uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1abqeng</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Can I use holo powder over a gel top coat?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abqeng/can_i_use_holo_powder_over_a_gel_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1abqbzb</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>Pearl 😍 to match with all the snow</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/er919emo3uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1abpyl1</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Early vday nails❣️</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/42yhuzwv0uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1abpkjm</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Mardi Gras nails!</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/yixn608oxtec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1abpolf</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>I dont have the nicest of fingers but nevertheless what do ya'll think?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4vpm80bpytec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1abpf2z</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t>Is there another way to go from nude/neutral to color other than ombre and French?</t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abpf2z/is_there_another_way_to_go_from_nudeneutral_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1abo0we</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>Why are my nails nearly clear? Can I keep them long or should I cut them?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abo0we</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1abp2he</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>When someone says they love your nails and you hit them with “thanks, I did them myself” and they’re like 😲</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbeq6mfyttec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1aboyva</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Natural Nails. Sheer Rosy Quartz</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aboyva</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1abor8u</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>One month and no chips! :)</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abor8u</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1aboemd</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>White nails:)</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7xz6msl3ptec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1aboeev</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>R.I.P. Tokyo a go-go! 😭</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sbhliie2ptec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1abobvb</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>V day mani :)</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abobvb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1abo43b</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>Valentines avant-garde</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9nsbo08xmtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1abo0d4</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t>This is my favorite set my friend did for me so far on my natural nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abo0d4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1abnspg</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>I like it 💅🏻. What do we think ?</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abnspg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1abnxej</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Short nails, trying to love them, will get there…</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fwrddaqfltec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1abnrba</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>Practice for my friends set tomorrow (inspo by @kessii.studio on insta)</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abnrba</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1abno4e</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>When you tell him how you feel and he decides to never speak to you again 🤡</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x2w8xtcijtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1abnf05</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t>Rubber Base Recommends</t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3f7jiy5nhtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1abjdrb</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>I want to remove my gelx and start building my natural nails— what is my best option?</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abjdrb/i_want_to_remove_my_gelx_and_start_building_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1ab7svs</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>Gel-X in New Jersey??</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ab7svs/gelx_in_new_jersey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1abmm2l</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>First time trying a V-French mani 😍</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3zmnajqqbtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1abmlqb</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>New set!</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abmlqb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1abmg1f</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Love me some iridescent powders</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q3dbfukgatec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1abm8ip</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>Do the accent nails look weird? Or fine?</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abm8ip</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1ablv15</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Did this new set on myself and I am proooooud!</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5kn0flc6tec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1abkvwd</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t>Baby blue nails💅🏻</t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4i2drp6uysec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1abkslg</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Calling these rose quartz nails 💕</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ftldmmy2ysec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1abitr0</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t>I already lost a rhinestone on my gem. What can I do?</t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abitr0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1abipde</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t>Black Winter</t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvl42flvgsec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1abidaa</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>First long set</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uooox6cxdsec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1abic4n</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>French tips</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psalq4rmdsec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1abi732</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>Second time gel painting, and aside from the edges, what do you think?</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1e003o7dcsec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1abhj21</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t>Valentines Nails!🌹😍🥰</t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8wghck1y5sec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1abhevq</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>Stamper pattern</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abhevq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1abh4e6</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>Photos before and after This girl loves rocks What do you think?</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abh4e6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1abh3wz</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Valentine’s Day 💘</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ef50y8iw1sec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1abg469</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>Tried a combination of acrylic dip &amp; gel x (mylee) to attach tips…very pleased with the result! Tutorial in comments</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t5o6nqv4rrec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1abfdel</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>My nail design for this sister’s wedding(her wedding dress is red and gold).</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abfdel</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1abdxcc</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>Got acrylics for the first time!</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8i1er3nzqec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1abdwrg</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>Am I ‚not made‘ for short nails?</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abdwrg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1abdpn0</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>and this color is my new passion, decided to share it with you</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cwknd0yowqec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1abdkfp</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>Decided to try this color and tell you the truth, I love it but wanna know your opinion about it</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e55z1a5puqec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1abdh7g</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Best at home nail kit for beginners?</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abdh7g/best_at_home_nail_kit_for_beginners/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1ac5sg9</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>In love with magnetic polish...</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2a690mghvxec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1ac55up</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t>Bluer than blue 💙🩵</t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac55up</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1ac45nu</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>Is anybody eyeing the Lurid Lacquer drop?</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ac45nu/is_anybody_eyeing_the_lurid_lacquer_drop/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1ac3ujh</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>On rare occasions I can convince myself that watermarbling is fun and that I ✨want✨ to do it</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac3ujh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1ac3hvy</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>🍋 in direct light</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1b77329c5xec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1ac3bcs</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>Mooncat Monster Under Your Head</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac3bcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1ac32zu</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Wide nails</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ac32zu/wide_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1ac2oyn</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>Blessed with Beauty and Rage</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8tooozuhxwec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1ac2p35</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>2nd air brush set!</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9h46jx4jxwec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1ac1ygs</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t>New here and to gel nails, need advice</t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ac1ygs/new_here_and_to_gel_nails_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1ac1cbq</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>A little self-care to end a chaotic week</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6dmypg6ekwec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1ac0rws</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>First Bees Knees Lacquer wear</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0rws</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1ac0lc5</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>Aquamarine by Cirque Colors 🌊</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0lc5</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1ac0k6f</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t>Mooncat, not all that.....</t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0k6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1ac0gc0</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>My favorite colour combo!</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0gc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1abzsgd</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>About to start learning how to do my own nails so my fiancé let me practice on him for the first time as a Guinea pig 😂</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abzsgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1abzfun</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>Penelope Luz Perfect Love</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/26wsffc43wec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1abzeov</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Had to repurchase Featured Guest after shattering my first bottle all over my nail bag 😭</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x3i2cctu2wec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1abym3w</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Mixed tone “neutral” mani</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4eraxzbwvvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1aby3sh</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t>First time using decals---kinda cute!</t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aby3sh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1abxzfq</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>matching my nails with my new fountain pen</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abxzfq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1abxxyi</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>thickening nail polish?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abxxyi/thickening_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1abxxmv</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>Pixie Party in the late afternoon sun.</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vu8axpl5qvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1abx8lc</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Nail colour dupe</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abx8lc/nail_colour_dupe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1abx0vh</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>Multichrome mani for the week</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abx0vh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1abwzln</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>Ethereal Snow Globe Mysteries</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abwzln</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1abweje</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>A little dark and moody before the valentines nails! Inspired by all the two finger skittles with “similar” colors</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abweje</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1abvzwv</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t>Ethereal— Transience</t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abvzwv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1abvnm2</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t>Help me find a polish to match!</t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abvnm2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1abvc3l</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>Way more excited than a person should be for this polish! Yooperlite!</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abvc3l</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1abuy0j</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t>Where to sell large collection of stamping polish/plates/accessories?</t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abuy0j/where_to_sell_large_collection_of_stamping/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1abut6f</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>LynB Lovelies from This Week</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abut6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1abul96</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>A not-quite-spring skittle 💕</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4m3iz5zrzuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1abug78</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t>New polish</t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abug78</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1abudo9</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Holo Taco - Bring me the Teal and Starry-Eyed</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/isoru397yuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1abudft</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t>My first time trying ILNP!</t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abudft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1abucot</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t>Nail beds can grow back!</t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jsdk80xzxuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1abu024</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Finally found the perfect burnt orange creme! 🥺🧡</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5uyqenjfvuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1abtt22</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>A shifty color dream</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abtt22</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1abthkw</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t>Wonka Skittle</t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cpaiwnkkruec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1abt5g2</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>{PR} Kiss Me Not by Krisable Designs</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zpqgj6lyouec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1absrtm</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>This polish makes it difficult to keep your eyes on the road 😉</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://imgur.com/gallery/tQwZJ0N</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1absr11</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Amazing Deal on Pop-Arazzi polish at CVS right now!</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1absr11</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1absfjz</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Can’t open bottles</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1absfjz/cant_open_bottles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1abs6dk</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t>Uses for nail clips?</t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cdqoi8vmhuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1abs1ok</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t>Polish Haul!</t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wxl86dfoguec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1abrrj9</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>Capricorn ♑️ 🐐</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abrrj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1abroai</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>Medication is making my nails peel. Any tips?</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abroai/medication_is_making_my_nails_peel_any_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1abrn6u</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>[Magnetic] Some fun magnet experimentation</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/Z6wlH2B</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1abr2ph</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Gold veins in quartz ✨💛</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abr2ph</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1abqrhn</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Like crystals ✨</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abqrhn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1abpwgn</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t>What are everyone's favourite pale, ghostly, gothic and ethereal Polish colours?</t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abpwgn/what_are_everyones_favourite_pale_ghostly_gothic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1abp94z</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>Looking for a dupe!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/es7kg3tdvtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1abp3af</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>When someone says they love your nails and you hit them with “thanks, I did them myself” and they’re like 😲</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6cf1ck24utec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1aboxi0</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Dupe for Julep - Fazia</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6j7ujj1xstec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1aboj25</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>First time using jelly nail polish</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z6ucy1d1qtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1abodlp</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t>questions about rubber base and led lamps!</t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abodlp/questions_about_rubber_base_and_led_lamps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1aboara</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Not great with magnetics…</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aboara</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1abo5yq</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t>New colors!</t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abo5yq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1abnmx0</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>Another gel set from Korea - I didn’t like the color combination as much but I polished over it with regular polish and love it so much more! In love with the 3D!</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abnmx0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1abnltt</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Coronation (2023 version)</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7iayyyv0jtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1abmt0c</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t>Noooooooooooo</t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abmt0c/noooooooooooo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1abmfjz</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>How to restore pushed cuticles back to original after manicurist ruined them?</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abmfjz/how_to_restore_pushed_cuticles_back_to_original/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1abm7x1</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Sharing my everyday color for the other basic ladies out there...but possible shrinkage problem</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abm7x1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1abm0e3</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>Which color??</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7aki8mxd7tec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1ablw0k</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t>Should I reshape?</t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ablw0k</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1abl19x</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>How do I keep my matte nails last longer?</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abl19x/how_do_i_keep_my_matte_nails_last_longer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1abkphq</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Match made in heaven</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abkphq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1abkbvp</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Does anyone else get name ick and won’t purchase a polish based on its name?</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abkbvp/does_anyone_else_get_name_ick_and_wont_purchase_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1abjcw4</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Another fun thermal :’)</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abjcw4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1abjbcx</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t>I wanted to like her…</t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5mqw033msec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1abigwg</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>Strawberry milkshake</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abigwg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1abhaps</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>Refreshing last week's mani</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzyl60wt3sec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1abgutz</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>What caused my nail to be at a right angle?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abgutz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1abfhws</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t>Is Salon Perfect 'Cosmic Dust' discontinued?</t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1abfhws/is_salon_perfect_cosmic_dust_discontinued/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1abfh79</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Dazzled</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abfh79</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1abemlg</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t>Tips on how to apply a glitter polish thinner in a small area?</t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abemlg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1ac24zy</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Beginner Press on resources</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1ac24zy/beginner_press_on_resources/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1ac0pfx</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Death Valley Maximalism</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0pfx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1ac0e1j</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t>In love with this colour combo</t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac0e1j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1abydbw</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>mid January</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abydbw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1abxx97</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>My latest set as a WA nail tech. ACOTAR inspired. IYKYK. 🥰🤍🏔️ @jolley.nails</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p6h8zmf2qvec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1abullq</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Valentine’s set by me 🎀 still improving!!</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ckjr22uuzuec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1abufgi</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>Valentine's Day Inspired Set</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v8i9l8qkyuec1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1abtlx2</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>Got bored</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abtlx2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1abssel</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>January Nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ic08tah9muec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1absos1</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>New nails for my best friend</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9kb49e7hluec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1absg9q</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t>Gave my sister a manicure 🌸</t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1absg9q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1abr5pg</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>will get as many aesthetic photos of my nails as much as I can before I need to get a full !! ( candy cream matte finished look ) done in Ontario at Chichi nails salon 🍭</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m489l7ry9uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1abq7u1</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t>Snake 🐍</t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6kexftss2uec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1abpn1l</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t>Bloody valentine ❤️</t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/womrnn4dytec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1abnoic</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>🤡</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fn0xmz7ljtec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1abne2v</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t>I absolutely love it</t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abne2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1abio86</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>Black winter</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pe7f1ixlgsec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1abfdm0</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t>My nail design for this sister’s wedding(her wedding dress is red and gold).</t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abfdm0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 28 08:07:57 UTC 2024
</commit_message>
<xml_diff>
--- a/data/2024_01_28.xlsx
+++ b/data/2024_01_28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1149"/>
+  <dimension ref="A1:C1329"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19966,6 +19966,3066 @@
         </is>
       </c>
     </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1acxdhd</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>First mani to show off my engagement ring 😍💍</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k4xfuyorx4fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1acx8r2</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Shortened the length? Do they suit?</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acx8r2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1acx78n</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t>Sailor Moon nails for my upcoming trip to Japan 🌙</t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acx78n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1acx404</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>pompompurin nails 💛</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lpg2djtju4fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1acwtmd</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>My new nail set 💅🏻 by @Piopionails ♒️🫶🏻💜</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acwtmd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1acwluv</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Went in for a fill. My color is amazing but..</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acwluv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1acwiar</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Steered away from traditional pink or red nails for Valentines. 🤭 Application is still sloppy but getting better from previous DIYs. 😊</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acwiar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1acwexw</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Just started doing my own nails a few months ago!</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acwexw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1acuhik</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t>Mistook regular color polish for gel</t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acuhik/mistook_regular_color_polish_for_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1acpn9j</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Suggestions to improve please</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vyp6su3mt2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1acpuya</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>inspired by pinterest, is it a good design for a wedding? as a guest thank you</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jork0dffv2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1acpz8x</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t>inspo was rainbow road from mario kart 🥰</t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/tgc5333hw2fc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1acq667</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>The Inspiration vs The Results</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acq667</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1acqk26</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t>New Set (First time post)</t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acqk26</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1acuj9v</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>Poyo~</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acuj9v</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1acvm04</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Valentines Nails</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekij7x3vd4fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1acw7ju</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>How does this happen?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x92kxanck4fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1acw0ys</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>nail tech essentials?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acw0ys/nail_tech_essentials/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1acvjwi</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t>I got my nails done today and my tech insisted on doing French tip this way but the extensions are clear?? Does this not look bad? Not trying to be rude at all I just don’t get it.</t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acvjwi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1acvh7w</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I’ve been getting good at doing my own acrylics and dip nails but this chunky glitter gave me a tough time</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acvh7w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1ace6lu</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t>First Time Extension Advice</t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ace6lu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1acapts</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>A small beautiful step towards a long coffin shape on natural nails</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acapts</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1ac821n</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Can I ask my nail artist to choose the design? How do I do that?</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ac821n/can_i_ask_my_nail_artist_to_choose_the_design_how/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1ac3yhx</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t>Can I get my nail art redone?</t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1ac3yhx/can_i_get_my_nail_art_redone/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1acu5rv</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t>I have super tiny nail beds for some reason. What types of nails do people with small nail beds buy?</t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acu5rv/i_have_super_tiny_nail_beds_for_some_reason_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1acu5mg</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t>What do you think??</t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/f6cmh95xy3fc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1actscv</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Had to share these babies 🤩🤩</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/0tu039y6v3fc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1actf00</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>first time</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ihzinynnr3fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1acsv5e</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>Still getting the hang of nail stickers</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acsv5e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1acrpbm</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Made my first press ons</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y6wtixjsb3fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1acr4kb</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>HELP: Got my nails done but the salon’s tools weren’t sanitized</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acr4kb/help_got_my_nails_done_but_the_salons_tools/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1acqxu9</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>I did my own (man)icure today, how’d I do?</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/psiw1esu43fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1acqvrp</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Valentine's nails</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/77jp5bpb43fc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1acqmf6</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>Tech’s Choice</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jluw3jw023fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1acqk5k</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>Tried grey this time</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pew8yc2h13fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1acqei4</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t>French times</t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acqei4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1acpy0i</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t>Color Chrome nails</t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acpy0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1acpwk3</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>My contribution to Valentine’s Day nails (I planned them to be more pink 😬)</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/84g0y2ctv2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1acpqal</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t>Did my own nails for the first time.</t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4kednribu2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1acpkcg</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Nail techs, is it true that...</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acpkcg/nail_techs_is_it_true_that/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1acou46</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Strongest Nail Glue</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acou46/strongest_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1acorm6</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>First time getting this shape. Wondering if it suits me.</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1ktsl29m2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1aco6cc</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>nothing sticks to my nails?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aco6cc/nothing_sticks_to_my_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1acnt82</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>How do we feel about milky polish?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acnt82</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1acnrww</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t>Press on nail advice</t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acnrww/press_on_nail_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1acnfgd</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t>Pretty happy with this hard gel</t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ldznrlqnb2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1acn5j3</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>Kur nail concealers are so ridiculously easy to use, it’s crazy! I applied this yesterday, literally in the dark! They typically last 10 days for me. I know it’s far from perfect but for a 2 min nail job without paying attention, I am really happy!</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acn5j3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1acmy55</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62mrdtzu72fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1acmq46</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t>Little grown out but I love this set!! 💅🏾👛🎀</t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ko2ou0s162fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1acmjfp</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Just love these!!</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u98kbb2m42fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1acmhqz</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Every once in a while a get the urge to turn my nails into a pocket ant farm.</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ke1jrsq842fc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1acmb0p</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t>Orange is my favorite color 🧡</t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yh5njxur22fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1acm4bq</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t>Winter blue!</t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s0v8qg0c12fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1aclu9y</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>TROUT NAILS 🦈🐡🎣🐠🐟</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aclu9y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1aclse3</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Valentines nails are on 😍</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fbjlq0ery1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1acbrr9</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Abstract Anime inspired nails!</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acbrr9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1accjs3</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t>Nails that match my hair ♥️</t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1accjs3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1ach0kd</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>How do I fix my nails after 25 years of nail biting?</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ach0kd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1aci9ih</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Opinions on my Pokemon (Espeon) nails?</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aci9ih</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1aclcns</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Cuticle oil enthusiasts! How quickly do you finish a bottle / tube?</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aclcns/cuticle_oil_enthusiasts_how_quickly_do_you_finish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1acizn3</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Got my nails done yesterday and realized they are way too long for me. How do I fix the length without ruining them??</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdzrhmyjc1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1ackxjz</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Flaming Hearts 💕</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vmwpxolkr1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1ackui8</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set 💕 what do you think?</t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ackui8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1ackow4</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>Help! I just did these lazy girl polygel and stained one with liquid wax dye 😭</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ackow4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1ackg7z</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Simple yet effective!</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qgamb9lwn1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1ack98v</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Obsessed ✨</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/binya60em1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1ack725</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>Milk Bath</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/29js37dxl1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1acjjd7</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>My New Nails</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5u0ouosg1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1acjiem</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t>I am blown AWAY by my nails. I’m never going to another tech.</t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acjiem</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1acjdxc</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t>New Nails</t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zxelbb3of1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1acjd8r</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t>🦩 Flaminglow 🧡 My first Cirque purchase. Picked up the Cirque Colors x Kelli Marissa Vegas Collection on clearance ✨</t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acjd8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1acjc3m</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t>I will never get bored of glazed nails</t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imwz843af1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1aciwnd</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Beginner gel kit?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aciwnd/beginner_gel_kit/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1acigmj</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t>Failed attempt at a subtle transition into Valentine’s Day</t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/682w5owe81fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1aciajp</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>How hard is DIY powder, really?</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1aciajp/how_hard_is_diy_powder_really/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1aci6ys</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>Nail Stickers</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aci6ys</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1aci6ve</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>I'm happy with how these are growing out</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aci6ve</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1achqbr</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>Help</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fdinwpgq21fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1ach5cf</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>I wanted to try something new, so I asked my nail tech for builder gel. I wanted to show them off because I think they turned out so good!</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h7m22dv8y0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1acgwxe</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t>Did my own acrylics for the first time</t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acgwxe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1acga31</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Weak nails</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acga31/weak_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1abw30e</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Gel and UV polish pops right off</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1abw30e/gel_and_uv_polish_pops_right_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1abuytv</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>V-day diy mani</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1abuytv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1acg6nl</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t>Fresh nails are my favourite way to celebrate a birthday 🥳</t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acg6nl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1acfwfg</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>First time ever trying press ons</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acfwfg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1acfog3</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t>Glitter + Hello Kitty💅</t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a0wc2f9wm0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1acfaor</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Jungle cat eye</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4xjmqyhwj0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1acf3wu</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>I like to do different designs on both hands, now i'm having silver vibes</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acf3wu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1acedkh</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t>Magical Unicorn Realness 🦄</t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/akycx3btc0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1acebrj</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t>I’m obsessed with this set I did</t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/srcu5ebfc0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1acdzj2</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>I love these 💜</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1cwwc4is90fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1acdy8v</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>Got to do these beautiful Swarovski frenchies yesterday! So happy w the outcome ❤️</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u50y8ukj90fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1acd9yp</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t>Got my nails did my mom is awesome!</t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/naqd4al540fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1acd9wg</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t>Cats eye amethyst Aquarius nails.</t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9zru0a7540fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1acd4oi</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t>What’s the best product to take off dip?</t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acd4oi/whats_the_best_product_to_take_off_dip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1accx1e</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t>Kicking off the Valentine’s Day vibes with some sweet cherries</t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikpcm1f610fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1acc1tg</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>First time gel nails</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acc1tg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1acbqa3</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t>Rate my new look! Went for something way different this time</t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zzgp96uwqzec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1acbi5h</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>Something shiny and colourful I did to survive the rest of this winter</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u246feruozec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1acbegv</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>How hard is it to do your own acrylics?</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1acbegv/how_hard_is_it_to_do_your_own_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1acx0td</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>New to getting my nails done and to BIAB - is it supposed to look like this?</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acx0td</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1acw9qz</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>bubbles in jelly polish?</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7swp8vm0l4fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1acw16n</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t>playing around with polish!</t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acw16n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1acvjcz</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t>Help! I absolutely cannot choose between matte or glossy.</t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acvjcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1acd3bm</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t>First magnetic attempt</t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0sinbxhm20fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1acuqlj</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>Dudley Nudshite!</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acuqlj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1actev5</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>ILNP Peace holographic</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yrbbsf0mr3fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1act1ke</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t>Hot pink and grey is my new favorite combo</t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fax40r55o3fc1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1acswia</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t>ILNP Rosewater ft. my cat 🌹 ✨️🐾</t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acswia</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1acslxf</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>Mixing jellies and aiming for Detroit Lion. Ended up a bit Tar Heel.</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kbykynp3k3fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1acsfhg</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t>How to make this pattern with magnetic polishes?</t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bzzrdbahi3fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1acs01t</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Should I use ridge filler?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acs01t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1acqkv3</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t>Tech’s Choice</t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/24z6dhan13fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1acqjcm</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>This is like an acid trip</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acqjcm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1acpswq</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t>Recommendations for nude/sheer nude polishes with a little ✨something extra✨?</t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acpswq/recommendations_for_nudesheer_nude_polishes_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1acpm1i</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Mooncat's Mermaid Bait is ✨MAGIC✨</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ir0ya8vbt2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1acp9ky</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Just wanted to share this pretty iridescent nail colour i put on my nails!</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4amoeaddq2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1acokdy</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Non gel silver, pink magnetic?</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acokdy/non_gel_silver_pink_magnetic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1acoi4s</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>I absolutely hate the thin brushes that come in cirque colors polishes. It seems like the wider brushes are always sold out. Have you tried using other brands wide brushes in cirque bottles?</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acoi4s/i_absolutely_hate_the_thin_brushes_that_come_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1acoi2f</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>Yard sale finds!</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acoi2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1aco1tr</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Gold or silver? 🍃</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aco1tr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1acnw59</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Looking for a medium grey polish, suggestions?</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acnw59/looking_for_a_medium_grey_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1acnf0d</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Nail Stickers</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acnf0d</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1acmq59</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>Evil Eye for Greece</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acmq59</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1acmgye</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>Icy blue lit up by holo: BKL - How Many Lives Does This Guy Have</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acmgye</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1aclyde</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t>Glow in the dark 🌟</t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aclyde</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1acld0g</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>Best brand for linear holo?</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acld0g/best_brand_for_linear_holo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1aclbi7</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Best handsoap for manicured nails?</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1aclbi7/best_handsoap_for_manicured_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1ackyt3</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t>Help, my uv polish falls off</t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ackyt3/help_my_uv_polish_falls_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1acky5w</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>First full hand crème in a long time</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5sxorsmqr1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1ackrxq</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>The Mist by a England. Question in caption</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g6pl6zqgq1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1ackh27</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>❄️🦉Snowy Owl🦉❄️</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ackh27</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1ack44c</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>Day 4 of Space Oddity; Give me Cuticle Advice!</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ack44c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1ack8c5</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>Polished for Days soft focus base coat</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ack8c5/polished_for_days_soft_focus_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1ack6y2</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Essie Here to Stay?</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ack6y2/essie_here_to_stay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1ack0ya</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t>Looking Slick 💧</t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ack0ya</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1acjbzy</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>🦩Flaminglow 🧡 My first Cirque purchase. Picked up the Cirque Colors x Kelli Marissa Vegas Collection on clearance ✨</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acjbzy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1acilfp</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t>Practice run for a Universal Orlando family vacation in the spring. Do these give Slytherin vibes?</t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acilfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1acidgt</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Games on Games within Games</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acidgt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1aci758</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>Chaotic Birthday Mani ♒</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1aci758</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1achyou</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>These are freaking stunning together- Ethereal combo</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1achyou</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1achyl3</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>She's giving sliced Kalamata olives</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5idbo65j41fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1achmfu</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t>My version of the magnet holder (cat's eye)</t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1achmfu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1achm4m</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>When is a polish too old?</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1achm4m/when_is_a_polish_too_old/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1achl50</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>ILNP - Bouquet Toss</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1achl50</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1achh6w</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>Matched my nails to my dress (or vice versa, if I’m being honest).</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g1ymqpvr01fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1achgu1</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>OPI Princesses Rule!</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35jo4q5p01fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1achb8g</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Sassy Sauce Cock a Doodle Doom</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q9rl72aiz0fc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1ach298</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>The "O.K FINE!" mani 🙄</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/sRJTZHW</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1acgbf6</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>HELP! I’ve tried everything 😭</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4mskojzur0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1acfydd</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>How do you guys keep track of new releases?</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1acfydd/how_do_you_guys_keep_track_of_new_releases/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1acfldv</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>A little brightness on this positively dreary day</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/od7x6av8m0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1acfczo</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>BKL Game Playing Deviant</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tx29a0kak0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1acf8x6</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>Mooncat Moonjelly as a topper over Insomniac</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acf8x6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1acesgz</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>{Gifted} Super shimmer!</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6xme54p0g0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1ace8j7</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>Magical Unicorn Realness 🦄</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j1w01nxpb0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1ace1tq</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>Press on nails are super difficult come off! Questions.</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1ace1tq/press_on_nails_are_super_difficult_come_off/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1acdzb5</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>The plan was to try the ♡ hack - failed completely, so went with that</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a19gcjvq90fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1acczxm</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Organized my current polish collection</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hxsd8iet10fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1accyhx</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Deep Red Skittle</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1accyhx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1accokd</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t>I wanted to use all my boyfriend's birthday gift to me</t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1accokd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1acc5yl</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Looking for a dupe for this burple-ish shade - Nitro Lacquer #045</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acc5yl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1acbv3g</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>Though Tuesday</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://imgur.com/a/8Jw9Rw0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1acb2u6</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>What are some of your favorite magnetic nail polishes?</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hk6pyg9hjzec1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1ac9eka</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t>My thumb cracks in this same place every time and causes a break later on, how do I stop this?</t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0x543c1j3zec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1ac91fu</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t>Since we don't have snow outside in my area... I'm trying to summon it</t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac91fu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1ac67g6</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>messed up my nails and turned into a 3d fish scale thing??😂😂😂</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1ac67g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1acxlli</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>Honestly funny</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1swtr06j05fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1acvy2j</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Valentines Day Nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acvy2j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1acvexy</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Black coquette nails done by me 🙌</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1acvexy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1acugk8</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>I'm loving this set, I have an amazing nail tech! What are your thoughts? Katie Laverenz is incredible at her art, every time.</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y8jeyxa024fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1act74e</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t>how can i avoid gumming/smudging/streaking when doing multiple layers of regular polish for nail art?</t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1act74e/how_can_i_avoid_gummingsmudgingstreaking_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1act1ma</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>valentines beginner set 💗</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1act1ma</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1acp3xd</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t>Do you like the nails I made? capping gel with hand design</t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2hphnbv1p2fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1acp2l7</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t>Poly gel</t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1acp2l7/poly_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1ackeiu</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Simple Valentine’s Day nails ❤️</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jed6adwjn1fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1achhh0</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t>Magic ✨ How would you rate this work?</t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1achhh0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1acfc18</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>Liquid steel 🗡️ what do u think?</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z8woy4c9k0fc1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1ac9969</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>Real Flowers for a Wedding</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wgrjm5zw1zec1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1ac7qko</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t>My nail art work on her natural nails.</t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5c2t8yqgjyec1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>